<commit_message>
Screenshots attached to Extent report for failure cases
Screenshots attached to Extent report for failure cases
</commit_message>
<xml_diff>
--- a/src/main/java/com/cdp/InputFiles/CDPLogin.xlsx
+++ b/src/main/java/com/cdp/InputFiles/CDPLogin.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="345" windowWidth="20730" windowHeight="9705"/>
+    <workbookView xWindow="360" yWindow="345" windowWidth="20730" windowHeight="9705" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
     <sheet name="TestSteps" sheetId="2" r:id="rId2"/>
+    <sheet name="CDPLogin" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="97">
   <si>
     <t>Proceed_ON_FAIL</t>
   </si>
@@ -218,29 +219,105 @@
     <t>Input user name in User Name Field</t>
   </si>
   <si>
-    <t>pariscustomer</t>
-  </si>
-  <si>
     <t>Input password in password field</t>
   </si>
   <si>
     <t>Password</t>
   </si>
   <si>
-    <t>Test@123</t>
-  </si>
-  <si>
     <t>Click on Sign In button</t>
   </si>
   <si>
-    <t>WELCOME TO PARIS.COM</t>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>DSID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Expectedmsg</t>
+  </si>
+  <si>
+    <t>Correct_Data</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Execution_Time</t>
+  </si>
+  <si>
+    <t>DS01</t>
+  </si>
+  <si>
+    <t>DS02</t>
+  </si>
+  <si>
+    <t>DS03</t>
+  </si>
+  <si>
+    <t>DS04</t>
+  </si>
+  <si>
+    <t>DS05</t>
+  </si>
+  <si>
+    <t>col$Password</t>
+  </si>
+  <si>
+    <t>col$UserName</t>
+  </si>
+  <si>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>WELCOME TO POLAND</t>
+  </si>
+  <si>
+    <t>verifySignIn</t>
+  </si>
+  <si>
+    <t>verifyErrorMsg</t>
+  </si>
+  <si>
+    <t>validate verify sign in functionality</t>
+  </si>
+  <si>
+    <t>validate error message</t>
+  </si>
+  <si>
+    <t>col$Expectedmsg</t>
+  </si>
+  <si>
+    <t>TS14</t>
+  </si>
+  <si>
+    <t>TS15</t>
+  </si>
+  <si>
+    <t>Please enter password</t>
+  </si>
+  <si>
+    <t>Please check your login credentials</t>
+  </si>
+  <si>
+    <t>LoginAlerMessage</t>
+  </si>
+  <si>
+    <t>Please enter usernam</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -277,8 +354,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="41"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -301,6 +384,12 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="56"/>
+        <bgColor indexed="62"/>
       </patternFill>
     </fill>
   </fills>
@@ -389,7 +478,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -402,6 +491,10 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -767,7 +860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -817,8 +910,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1016,7 +1109,7 @@
         <v>50</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>3</v>
@@ -1120,7 +1213,7 @@
         <v>64</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>3</v>
@@ -1137,16 +1230,16 @@
         <v>37</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>41</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>3</v>
@@ -1163,7 +1256,7 @@
         <v>38</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>27</v>
@@ -1180,24 +1273,52 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="7"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="A15" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>86</v>
+      </c>
       <c r="E15" s="3"/>
       <c r="F15" s="11"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="8"/>
+      <c r="G15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="7"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="8"/>
+      <c r="A16" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" thickBot="1">
       <c r="A17" s="7" t="s">
@@ -1223,10 +1344,140 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="F13" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="257" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="257" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Test Case description added
Test Case description added
</commit_message>
<xml_diff>
--- a/src/main/java/com/cdp/InputFiles/CDPLogin.xlsx
+++ b/src/main/java/com/cdp/InputFiles/CDPLogin.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="96">
   <si>
     <t>Proceed_ON_FAIL</t>
   </si>
@@ -145,9 +145,6 @@
   </si>
   <si>
     <t>Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t xml:space="preserve"> Reset web application</t>
@@ -887,10 +884,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
         <v>44</v>
-      </c>
-      <c r="B2" t="s">
-        <v>45</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -911,7 +908,7 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -934,7 +931,7 @@
         <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>18</v>
@@ -954,7 +951,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>10</v>
@@ -976,7 +973,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>20</v>
@@ -988,7 +985,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
@@ -1000,7 +997,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>22</v>
@@ -1013,7 +1010,7 @@
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>3</v>
@@ -1024,7 +1021,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>25</v>
@@ -1046,19 +1043,19 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>26</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>33</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
@@ -1070,220 +1067,220 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>33</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>32</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>34</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>36</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>41</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>41</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>38</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>27</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F14" s="11"/>
       <c r="G14" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:8">
       <c r="A15" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="11"/>
@@ -1291,48 +1288,48 @@
         <v>3</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:8">
       <c r="A16" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="D16" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="G16" s="3" t="s">
         <v>3</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" thickBot="1">
       <c r="A17" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D17" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F17" s="9"/>
       <c r="G17" s="9" t="s">
@@ -1371,39 +1368,39 @@
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>72</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>73</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>16</v>
       </c>
       <c r="G1" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="12" t="s">
         <v>74</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
         <v>69</v>
-      </c>
-      <c r="C2" t="s">
-        <v>70</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>39</v>
@@ -1414,16 +1411,16 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F3" s="13" t="s">
         <v>39</v>
@@ -1431,16 +1428,16 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F4" s="13" t="s">
         <v>39</v>
@@ -1448,13 +1445,13 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>39</v>
@@ -1462,16 +1459,16 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E6" s="13" t="s">
         <v>83</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>84</v>
       </c>
       <c r="F6" s="13" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
fixed extent report description issue
</commit_message>
<xml_diff>
--- a/src/main/java/com/cdp/InputFiles/CDPLogin.xlsx
+++ b/src/main/java/com/cdp/InputFiles/CDPLogin.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="345" windowWidth="20730" windowHeight="9705" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="345" windowWidth="20730" windowHeight="9705" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -907,7 +907,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -1350,8 +1350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>